<commit_message>
use consistent error messages
</commit_message>
<xml_diff>
--- a/data/epp-09-status-data.xlsx
+++ b/data/epp-09-status-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/icann/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79B484B-26D1-D844-BB82-F3848A25F92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F493E7-118A-764F-8651-8A98496F868E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="16860" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -738,7 +738,7 @@
   <dimension ref="B2:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
move rem clientUpdateProhibited test so other tests work
</commit_message>
<xml_diff>
--- a/data/epp-09-status-data.xlsx
+++ b/data/epp-09-status-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E721793-5CCB-B443-955C-4E0A77FC7204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18B1F6F-DEDB-0640-A698-982A6204BA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="16860" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
   <dimension ref="B2:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -856,10 +856,10 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
@@ -876,10 +876,10 @@
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
@@ -887,13 +887,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
@@ -901,7 +901,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -915,7 +915,7 @@
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1</v>
@@ -929,7 +929,7 @@
         <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
@@ -943,7 +943,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
@@ -957,7 +957,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
@@ -971,7 +971,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>1</v>
@@ -985,7 +985,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>1</v>
@@ -999,7 +999,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>1</v>
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>1</v>
@@ -1024,16 +1024,16 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>